<commit_message>
Update of Excel files
</commit_message>
<xml_diff>
--- a/Pair 1 - Jaskaran & William/TuTh1045to12-Group1Pair1-GanttHW2.xlsx
+++ b/Pair 1 - Jaskaran & William/TuTh1045to12-Group1Pair1-GanttHW2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaskaran/Documents/GitHub/CSCI331Group1/Pair 1 - Jaskaran &amp; William/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5A61134-57CE-F346-8F46-0183950DA357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BE7FE2-74D2-3846-BBA2-49DA952196C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -667,120 +667,7 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -1170,7 +1057,7 @@
   <dimension ref="B1:BO30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="108" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1508,7 +1395,7 @@
         <v>39</v>
       </c>
       <c r="C6" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" s="7">
         <v>2</v>
@@ -1528,13 +1415,13 @@
         <v>35</v>
       </c>
       <c r="C7" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
       </c>
       <c r="E7" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -1548,16 +1435,16 @@
         <v>36</v>
       </c>
       <c r="C8" s="7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" s="7">
         <v>2</v>
       </c>
       <c r="E8" s="7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F8" s="7">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G8" s="8">
         <v>0.1</v>
@@ -1568,13 +1455,13 @@
         <v>37</v>
       </c>
       <c r="C9" s="7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="E9" s="7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F9" s="7">
         <v>1</v>
@@ -1588,13 +1475,13 @@
         <v>40</v>
       </c>
       <c r="C10" s="7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="E10" s="7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F10" s="7">
         <v>1</v>
@@ -2019,38 +1906,38 @@
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="B31:BO31">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="16" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:BO30">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="1" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="0" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>